<commit_message>
Cambios en la base de datos, version 2.4
</commit_message>
<xml_diff>
--- a/recursos/esquema_uisrael_ejemplo.xlsx
+++ b/recursos/esquema_uisrael_ejemplo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rafael\Dropbox\asistencia_uisrael\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Dropbox\asistencia_uisrael\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="2070" windowWidth="20490" windowHeight="9630" tabRatio="798" firstSheet="6" activeTab="19"/>
+    <workbookView xWindow="5070" yWindow="2070" windowWidth="20490" windowHeight="9630" tabRatio="798" firstSheet="8" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="area_conocimiento" sheetId="22" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <sheet name="curso" sheetId="8" r:id="rId10"/>
     <sheet name="semana" sheetId="11" r:id="rId11"/>
     <sheet name="tematica" sheetId="12" r:id="rId12"/>
-    <sheet name="silabo_detalle" sheetId="10" r:id="rId13"/>
-    <sheet name="curso_aperturado" sheetId="13" r:id="rId14"/>
-    <sheet name="modalidad" sheetId="14" r:id="rId15"/>
-    <sheet name="aula" sheetId="15" r:id="rId16"/>
-    <sheet name="seccion" sheetId="16" r:id="rId17"/>
-    <sheet name="carga_academica" sheetId="18" r:id="rId18"/>
+    <sheet name="curso_aperturado" sheetId="13" r:id="rId13"/>
+    <sheet name="modalidad" sheetId="14" r:id="rId14"/>
+    <sheet name="aula" sheetId="15" r:id="rId15"/>
+    <sheet name="seccion" sheetId="16" r:id="rId16"/>
+    <sheet name="carga_academica" sheetId="18" r:id="rId17"/>
+    <sheet name="silabo_detalle" sheetId="10" r:id="rId18"/>
     <sheet name="dia_semana" sheetId="19" r:id="rId19"/>
     <sheet name="horario" sheetId="20" r:id="rId20"/>
     <sheet name="matricula" sheetId="21" r:id="rId21"/>
@@ -5699,514 +5699,6 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>869</v>
-      </c>
-      <c r="C2" s="13">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>869</v>
-      </c>
-      <c r="C3" s="13">
-        <v>2</v>
-      </c>
-      <c r="D3" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>869</v>
-      </c>
-      <c r="C4" s="13">
-        <v>3</v>
-      </c>
-      <c r="D4" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>869</v>
-      </c>
-      <c r="C5" s="13">
-        <v>4</v>
-      </c>
-      <c r="D5" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
-        <v>869</v>
-      </c>
-      <c r="C6" s="13">
-        <v>5</v>
-      </c>
-      <c r="D6" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>869</v>
-      </c>
-      <c r="C7" s="13">
-        <v>6</v>
-      </c>
-      <c r="D7" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>869</v>
-      </c>
-      <c r="C8" s="13">
-        <v>7</v>
-      </c>
-      <c r="D8" s="13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>869</v>
-      </c>
-      <c r="C9" s="13">
-        <v>8</v>
-      </c>
-      <c r="D9" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>869</v>
-      </c>
-      <c r="C10" s="13">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>869</v>
-      </c>
-      <c r="C11" s="13">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>869</v>
-      </c>
-      <c r="C12" s="13">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>869</v>
-      </c>
-      <c r="C13" s="13">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>869</v>
-      </c>
-      <c r="C14" s="13">
-        <v>13</v>
-      </c>
-      <c r="D14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>869</v>
-      </c>
-      <c r="C15" s="13">
-        <v>14</v>
-      </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>869</v>
-      </c>
-      <c r="C16" s="13">
-        <v>15</v>
-      </c>
-      <c r="D16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>869</v>
-      </c>
-      <c r="C17" s="13">
-        <v>16</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>869</v>
-      </c>
-      <c r="C18" s="13">
-        <v>17</v>
-      </c>
-      <c r="D18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>870</v>
-      </c>
-      <c r="C19" s="13">
-        <v>1</v>
-      </c>
-      <c r="D19" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
-        <v>870</v>
-      </c>
-      <c r="C20" s="13">
-        <v>2</v>
-      </c>
-      <c r="D20" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1">
-        <v>870</v>
-      </c>
-      <c r="C21" s="13">
-        <v>3</v>
-      </c>
-      <c r="D21" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1">
-        <v>870</v>
-      </c>
-      <c r="C22" s="13">
-        <v>4</v>
-      </c>
-      <c r="D22" s="13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1">
-        <v>870</v>
-      </c>
-      <c r="C23" s="13">
-        <v>5</v>
-      </c>
-      <c r="D23" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1">
-        <v>870</v>
-      </c>
-      <c r="C24" s="13">
-        <v>6</v>
-      </c>
-      <c r="D24" s="13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1">
-        <v>870</v>
-      </c>
-      <c r="C25" s="13">
-        <v>7</v>
-      </c>
-      <c r="D25" s="13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>870</v>
-      </c>
-      <c r="C26" s="13">
-        <v>8</v>
-      </c>
-      <c r="D26" s="13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1">
-        <v>870</v>
-      </c>
-      <c r="C27" s="13">
-        <v>9</v>
-      </c>
-      <c r="D27" s="13">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1">
-        <v>870</v>
-      </c>
-      <c r="C28" s="13">
-        <v>10</v>
-      </c>
-      <c r="D28" s="13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>870</v>
-      </c>
-      <c r="C29" s="13">
-        <v>11</v>
-      </c>
-      <c r="D29" s="13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1">
-        <v>870</v>
-      </c>
-      <c r="C30" s="13">
-        <v>12</v>
-      </c>
-      <c r="D30" s="13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1">
-        <v>870</v>
-      </c>
-      <c r="C31" s="13">
-        <v>13</v>
-      </c>
-      <c r="D31" s="13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
-        <v>870</v>
-      </c>
-      <c r="C32" s="13">
-        <v>14</v>
-      </c>
-      <c r="D32" s="13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>870</v>
-      </c>
-      <c r="C33" s="13">
-        <v>15</v>
-      </c>
-      <c r="D33" s="13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1">
-        <v>870</v>
-      </c>
-      <c r="C34" s="13">
-        <v>16</v>
-      </c>
-      <c r="D34" s="13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1">
-        <v>870</v>
-      </c>
-      <c r="C35" s="13">
-        <v>17</v>
-      </c>
-      <c r="D35" s="13">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7449,7 +6941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -7500,7 +6992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -7543,7 +7035,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -7590,12 +7082,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="A1:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7779,6 +7271,514 @@
       </c>
       <c r="K5">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>869</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>869</v>
+      </c>
+      <c r="C3" s="13">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>869</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3</v>
+      </c>
+      <c r="D4" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>869</v>
+      </c>
+      <c r="C5" s="13">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>869</v>
+      </c>
+      <c r="C6" s="13">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>869</v>
+      </c>
+      <c r="C7" s="13">
+        <v>6</v>
+      </c>
+      <c r="D7" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>869</v>
+      </c>
+      <c r="C8" s="13">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>869</v>
+      </c>
+      <c r="C9" s="13">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>869</v>
+      </c>
+      <c r="C10" s="13">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>869</v>
+      </c>
+      <c r="C11" s="13">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>869</v>
+      </c>
+      <c r="C12" s="13">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>869</v>
+      </c>
+      <c r="C13" s="13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>869</v>
+      </c>
+      <c r="C14" s="13">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>869</v>
+      </c>
+      <c r="C15" s="13">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>869</v>
+      </c>
+      <c r="C16" s="13">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>869</v>
+      </c>
+      <c r="C17" s="13">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>869</v>
+      </c>
+      <c r="C18" s="13">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>870</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>870</v>
+      </c>
+      <c r="C20" s="13">
+        <v>2</v>
+      </c>
+      <c r="D20" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>870</v>
+      </c>
+      <c r="C21" s="13">
+        <v>3</v>
+      </c>
+      <c r="D21" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>870</v>
+      </c>
+      <c r="C22" s="13">
+        <v>4</v>
+      </c>
+      <c r="D22" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>870</v>
+      </c>
+      <c r="C23" s="13">
+        <v>5</v>
+      </c>
+      <c r="D23" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>870</v>
+      </c>
+      <c r="C24" s="13">
+        <v>6</v>
+      </c>
+      <c r="D24" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>870</v>
+      </c>
+      <c r="C25" s="13">
+        <v>7</v>
+      </c>
+      <c r="D25" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>870</v>
+      </c>
+      <c r="C26" s="13">
+        <v>8</v>
+      </c>
+      <c r="D26" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>870</v>
+      </c>
+      <c r="C27" s="13">
+        <v>9</v>
+      </c>
+      <c r="D27" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>870</v>
+      </c>
+      <c r="C28" s="13">
+        <v>10</v>
+      </c>
+      <c r="D28" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>870</v>
+      </c>
+      <c r="C29" s="13">
+        <v>11</v>
+      </c>
+      <c r="D29" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>870</v>
+      </c>
+      <c r="C30" s="13">
+        <v>12</v>
+      </c>
+      <c r="D30" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>870</v>
+      </c>
+      <c r="C31" s="13">
+        <v>13</v>
+      </c>
+      <c r="D31" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>870</v>
+      </c>
+      <c r="C32" s="13">
+        <v>14</v>
+      </c>
+      <c r="D32" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>870</v>
+      </c>
+      <c r="C33" s="13">
+        <v>15</v>
+      </c>
+      <c r="D33" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>870</v>
+      </c>
+      <c r="C34" s="13">
+        <v>16</v>
+      </c>
+      <c r="D34" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>870</v>
+      </c>
+      <c r="C35" s="13">
+        <v>17</v>
+      </c>
+      <c r="D35" s="13">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -8088,7 +8088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambios en la base de datos, version 2.4.1, Correcion de errores
</commit_message>
<xml_diff>
--- a/recursos/esquema_uisrael_ejemplo.xlsx
+++ b/recursos/esquema_uisrael_ejemplo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Dropbox\asistencia_uisrael\recursos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\asistencia_uisrael\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="2070" windowWidth="20490" windowHeight="9630" tabRatio="798" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="6000" yWindow="2070" windowWidth="20490" windowHeight="9630" tabRatio="821" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="area_conocimiento" sheetId="22" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="348">
   <si>
     <t>usuario</t>
   </si>
@@ -7086,7 +7086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -7280,509 +7280,616 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D35"/>
+      <selection activeCell="E35" sqref="A1:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="13">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
         <v>869</v>
-      </c>
-      <c r="C2" s="13">
-        <v>1</v>
       </c>
       <c r="D2" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="13">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
         <v>869</v>
-      </c>
-      <c r="C3" s="13">
-        <v>2</v>
       </c>
       <c r="D3" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="13">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
         <v>869</v>
-      </c>
-      <c r="C4" s="13">
-        <v>3</v>
       </c>
       <c r="D4" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="13">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1">
         <v>869</v>
-      </c>
-      <c r="C5" s="13">
-        <v>4</v>
       </c>
       <c r="D5" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="13">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
         <v>869</v>
-      </c>
-      <c r="C6" s="13">
-        <v>5</v>
       </c>
       <c r="D6" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="13">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
         <v>869</v>
-      </c>
-      <c r="C7" s="13">
-        <v>6</v>
       </c>
       <c r="D7" s="13">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="13">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
         <v>869</v>
-      </c>
-      <c r="C8" s="13">
-        <v>7</v>
       </c>
       <c r="D8" s="13">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="13">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
         <v>869</v>
-      </c>
-      <c r="C9" s="13">
-        <v>8</v>
       </c>
       <c r="D9" s="13">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="13">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>869</v>
       </c>
-      <c r="C10" s="13">
+      <c r="D10" s="13">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="13">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
         <v>869</v>
       </c>
-      <c r="C11" s="13">
+      <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="13">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
         <v>869</v>
       </c>
-      <c r="C12" s="13">
+      <c r="D12" s="13">
         <v>11</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
         <v>869</v>
       </c>
-      <c r="C13" s="13">
+      <c r="D13" s="13">
         <v>12</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="13">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
         <v>869</v>
       </c>
-      <c r="C14" s="13">
+      <c r="D14" s="13">
         <v>13</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="13">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
         <v>869</v>
       </c>
-      <c r="C15" s="13">
+      <c r="D15" s="13">
         <v>14</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="13">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1">
         <v>869</v>
       </c>
-      <c r="C16" s="13">
+      <c r="D16" s="13">
         <v>15</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="13">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1">
         <v>869</v>
       </c>
-      <c r="C17" s="13">
+      <c r="D17" s="13">
         <v>16</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="13">
+        <v>9</v>
+      </c>
+      <c r="C18" s="1">
         <v>869</v>
       </c>
-      <c r="C18" s="13">
+      <c r="D18" s="13">
         <v>17</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="13">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1">
         <v>870</v>
-      </c>
-      <c r="C19" s="13">
-        <v>1</v>
       </c>
       <c r="D19" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="13">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1">
         <v>870</v>
-      </c>
-      <c r="C20" s="13">
-        <v>2</v>
       </c>
       <c r="D20" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="13">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
         <v>870</v>
-      </c>
-      <c r="C21" s="13">
-        <v>3</v>
       </c>
       <c r="D21" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="13">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1">
         <v>870</v>
-      </c>
-      <c r="C22" s="13">
-        <v>4</v>
       </c>
       <c r="D22" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="13">
+        <v>9</v>
+      </c>
+      <c r="C23" s="1">
         <v>870</v>
-      </c>
-      <c r="C23" s="13">
-        <v>5</v>
       </c>
       <c r="D23" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="13">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1">
         <v>870</v>
-      </c>
-      <c r="C24" s="13">
-        <v>6</v>
       </c>
       <c r="D24" s="13">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="13">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1">
         <v>870</v>
-      </c>
-      <c r="C25" s="13">
-        <v>7</v>
       </c>
       <c r="D25" s="13">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="13">
+        <v>9</v>
+      </c>
+      <c r="C26" s="1">
         <v>870</v>
-      </c>
-      <c r="C26" s="13">
-        <v>8</v>
       </c>
       <c r="D26" s="13">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="13">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1">
         <v>870</v>
-      </c>
-      <c r="C27" s="13">
-        <v>9</v>
       </c>
       <c r="D27" s="13">
         <v>9</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="13">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1">
         <v>870</v>
-      </c>
-      <c r="C28" s="13">
-        <v>10</v>
       </c>
       <c r="D28" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="13">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1">
         <v>870</v>
-      </c>
-      <c r="C29" s="13">
-        <v>11</v>
       </c>
       <c r="D29" s="13">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="13">
+        <v>9</v>
+      </c>
+      <c r="C30" s="1">
         <v>870</v>
-      </c>
-      <c r="C30" s="13">
-        <v>12</v>
       </c>
       <c r="D30" s="13">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="13">
+        <v>9</v>
+      </c>
+      <c r="C31" s="1">
         <v>870</v>
-      </c>
-      <c r="C31" s="13">
-        <v>13</v>
       </c>
       <c r="D31" s="13">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="13">
+        <v>9</v>
+      </c>
+      <c r="C32" s="1">
         <v>870</v>
-      </c>
-      <c r="C32" s="13">
-        <v>14</v>
       </c>
       <c r="D32" s="13">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="13">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1">
         <v>870</v>
-      </c>
-      <c r="C33" s="13">
-        <v>15</v>
       </c>
       <c r="D33" s="13">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="13">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1">
         <v>870</v>
-      </c>
-      <c r="C34" s="13">
-        <v>16</v>
       </c>
       <c r="D34" s="13">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="13">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1">
         <v>870</v>
-      </c>
-      <c r="C35" s="13">
-        <v>17</v>
       </c>
       <c r="D35" s="13">
         <v>17</v>
       </c>
+      <c r="E35" s="13">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8866,7 +8973,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8906,8 +9013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>